<commit_message>
23153: Add DoD ID to test specimen fields
SVN r37656 |2015-04-23 01:27:49 +0000
</commit_message>
<xml_diff>
--- a/hdrl/resources/template/specimenTemplate.xlsx
+++ b/hdrl/resources/template/specimenTemplate.xlsx
@@ -31,9 +31,6 @@
     <t>SSN</t>
   </si>
   <si>
-    <t>Request</t>
-  </si>
-  <si>
     <t>FMP</t>
   </si>
   <si>
@@ -44,6 +41,9 @@
   </si>
   <si>
     <t>Draw Date</t>
+  </si>
+  <si>
+    <t>DOD Id</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD15"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -395,7 +395,7 @@
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
@@ -419,19 +419,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix to Issue 23490 : Middle name field not included in HDRL test request template
SVN r38323 |2015-06-10 19:35:23 +0000
</commit_message>
<xml_diff>
--- a/hdrl/resources/template/specimenTemplate.xlsx
+++ b/hdrl/resources/template/specimenTemplate.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="16935" windowHeight="6855"/>
+    <workbookView xWindow="400" yWindow="640" windowWidth="16940" windowHeight="6860"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Customer Barcode</t>
   </si>
@@ -44,13 +49,16 @@
   </si>
   <si>
     <t>DOD Id</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -380,29 +388,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -413,24 +422,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -439,5 +451,10 @@
   <headerFooter>
     <oddFooter>&amp;Cdata&amp;L&amp;D&amp;RPage &amp;P/&amp;N</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Spec 23373: Labware integration for request submission
SVN r38653 |2015-07-03 15:06:39 +0000
</commit_message>
<xml_diff>
--- a/hdrl/resources/template/specimenTemplate.xlsx
+++ b/hdrl/resources/template/specimenTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="640" windowWidth="16940" windowHeight="6860"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Customer Barcode</t>
   </si>
@@ -52,13 +52,19 @@
   </si>
   <si>
     <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Initials</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -70,6 +76,29 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,14 +118,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,11 +423,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -402,16 +436,16 @@
     <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,30 +458,37 @@
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;Cdata&amp;L&amp;D&amp;RPage &amp;P/&amp;N</oddFooter>
   </headerFooter>

</xml_diff>